<commit_message>
Add new data row in data_versions.csv
A new data row has been appended to the data_versions.csv file. This addition expands the dataset with current information and ensures its completeness.

Fixed a bug that loaded best_model.pkl instead of ml_model.pkl
</commit_message>
<xml_diff>
--- a/data description.xlsx
+++ b/data description.xlsx
@@ -1,31 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahima.Prasad\Downloads\Datasets (4)\Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0b75638021b19a6/Karriere/IT/Data Science Bootcamp/Final Project/HospitalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F65532-9386-4A4F-ADC6-5E3EB3C5E419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{F5F65532-9386-4A4F-ADC6-5E3EB3C5E419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D7AC5B5-7DDB-D746-A883-32844650A18D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t>Provider ID</t>
   </si>
@@ -370,13 +383,91 @@
   </si>
   <si>
     <t>Rating group of the hospital</t>
+  </si>
+  <si>
+    <t>dataset 1</t>
+  </si>
+  <si>
+    <t>dataset 2</t>
+  </si>
+  <si>
+    <t>dataset 3</t>
+  </si>
+  <si>
+    <t>feature 1</t>
+  </si>
+  <si>
+    <t>feature 2</t>
+  </si>
+  <si>
+    <t>feature 3</t>
+  </si>
+  <si>
+    <t>feature 4</t>
+  </si>
+  <si>
+    <t>feature 5</t>
+  </si>
+  <si>
+    <t>feature 6</t>
+  </si>
+  <si>
+    <t>feature 7</t>
+  </si>
+  <si>
+    <t>feature 8</t>
+  </si>
+  <si>
+    <t>feature 9</t>
+  </si>
+  <si>
+    <t>feature 10</t>
+  </si>
+  <si>
+    <t>feature 11</t>
+  </si>
+  <si>
+    <t>feature 12</t>
+  </si>
+  <si>
+    <t>feature 13</t>
+  </si>
+  <si>
+    <t>feature 14</t>
+  </si>
+  <si>
+    <t>feature 15</t>
+  </si>
+  <si>
+    <t>feature 16</t>
+  </si>
+  <si>
+    <t>feature 17</t>
+  </si>
+  <si>
+    <t>feature 18</t>
+  </si>
+  <si>
+    <t>feature 19</t>
+  </si>
+  <si>
+    <t>feature 20</t>
+  </si>
+  <si>
+    <t>feature 21</t>
+  </si>
+  <si>
+    <t>feature 22</t>
+  </si>
+  <si>
+    <t>feature 23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,6 +479,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -418,18 +515,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -710,75 +807,74 @@
   <dimension ref="A1:B95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="48.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -786,7 +882,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -794,7 +890,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -802,7 +898,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -810,7 +906,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -818,7 +914,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -826,7 +922,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -834,7 +930,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -842,7 +938,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -850,7 +946,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -858,45 +954,45 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -904,431 +1000,431 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="2"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="3"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="3"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="2"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B67" s="2"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B68" s="2"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B69" s="2"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B70" s="2"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="2"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B73" s="2"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="2"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B75" s="2"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B76" s="2"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B77" s="2"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B78" s="2"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B79" s="2"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B80" s="2"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="3"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B81" s="2"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B82" s="2"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="3"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B83" s="2"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B84" s="2"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B85" s="2"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="3"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B86" s="2"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="3"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B87" s="2"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="3"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B88" s="2"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="3"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B89" s="2"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="3"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="4"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="4"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="4"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B94" s="3"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B94" s="4"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B95" s="3"/>
+      <c r="B95" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1344,4 +1440,547 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABF1457-4ED9-1844-858F-B14D416A1941}">
+  <dimension ref="C1:F24"/>
+  <sheetViews>
+    <sheetView zoomScale="164" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2">
+        <f ca="1">RAND()</f>
+        <v>0.57668407506436625</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:F17" ca="1" si="0">RAND()</f>
+        <v>0.98348730497288739</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.53483846533941637</v>
+      </c>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:F24" ca="1" si="1">RAND()</f>
+        <v>0.85408051240576766</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.98978808135703289</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.33757919701292305</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.45754440242945571</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.52410341090008472</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.33387216517590024</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.7395573983801573E-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.75595138500499803</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.38514520555634357</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.0368836637862624E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.33922788361359002</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.66717810438231884</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.41592608734480363</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.20359043385487618</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.85855173845334165</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.23680004958624834</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.81764084793712488</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.40451582748464698</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.3302684857558279</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.78569144090427823</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.34799936708656021</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.60689810170916714</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12897121812537438</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.30015753583898663</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.87609463213671313</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.18567614118208575</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.82931627445216949</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.51091856892141752</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.85951601167703884</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.74909897795432379</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.50443841549343515</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.26043672763724635</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.53969516810944795</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.4921663832757428E-2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.85336774710585339</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.26451888441879001</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.22711581419930937</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.42680354605260185</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.94675398059190941</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.80892004902900094</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.6481576397380705</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4791177996186233E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.32991055122011159</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.85994667452854967</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.23278598317019117</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.3105214857022186</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.0753536974735853E-2</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.29829285012238604</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.57296505833956102</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9173099266180359</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.27870829636046168</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.2478155834772982E-2</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.83327894634211541</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.55121156151808537</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.86859464773401873</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.68089364379171979</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.99589919832442253</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.75307936008678322</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.80784083120232586</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.29420892887948247</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>140</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.85763267970943158</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.52260926178426148</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.89267146113977958</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="D2:F2">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{68440A6F-AD10-5546-9F77-41DDD0D390F4}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:F3">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{06C6E932-E073-9141-8D23-79AFEA985533}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:F4">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AC76CD70-1E64-5449-AA2C-4A885BA8AA06}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:F8">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EB656738-A915-994F-86EF-127F6118FCBB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{68440A6F-AD10-5546-9F77-41DDD0D390F4}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D2:F2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{06C6E932-E073-9141-8D23-79AFEA985533}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D3:F3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AC76CD70-1E64-5449-AA2C-4A885BA8AA06}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D4:F4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EB656738-A915-994F-86EF-127F6118FCBB}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D8:F8</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F97DA-32E7-014C-8A3B-322B02B89496}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>